<commit_message>
Se añaden los modulos para hacer el XML, subir el fichero PDF, subir el fichero XML, y cargar los datos del QueueItem en un diccionario, además de modificaciones en el fichero config.xlsx
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webersolutionsespana-my.sharepoint.com/personal/jgonzalez_rpatechnologies_es/Documents/Documentos/UiPath/AVO_001_0300_Exportar_Facturas/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12B07524-CC09-4E9A-A188-6B4D944687D2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -159,7 +156,25 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>AVO_001_0300_Exportar_Facturas</t>
+  </si>
+  <si>
+    <t>PDFDestinationPath</t>
+  </si>
+  <si>
+    <t>XMLDestinationPath</t>
+  </si>
+  <si>
+    <t>PDFOriginPath</t>
+  </si>
+  <si>
+    <t>Ruta donde se almacena el documento original de la factura</t>
+  </si>
+  <si>
+    <t>Ruta donde se almacenará el documento PDF en los sistemas del cliente</t>
+  </si>
+  <si>
+    <t>Ruta donde se almacenará el documento XML generado</t>
   </si>
 </sst>
 </file>
@@ -239,7 +254,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -537,19 +552,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,43 +598,66 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2"/>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1620,15 +1658,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1703,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1673,18 +1711,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1746,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1768,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1790,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,14 +2820,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +2840,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Se modifica el módulo CreateXML para generar directamente el fichero XML, se crea el fichero para generar la parte de XML que tendrá los distintos impuestos y se crea el código que creará las distintas líneas de la factura. Se crea el módulo para subir los archivos a FTP.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webersolutionsespana-my.sharepoint.com/personal/jgonzalez_rpatechnologies_es/Documents/Documentos/UiPath/AVO_001_0300_Exportar_Facturas/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12B07524-CC09-4E9A-A188-6B4D944687D2}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5700A415-4604-4AFA-A2D7-D48FB3662746}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -175,13 +175,37 @@
   </si>
   <si>
     <t>Ruta donde se almacenará el documento XML generado</t>
+  </si>
+  <si>
+    <t>SFTPHost</t>
+  </si>
+  <si>
+    <t>Host del cliente al que se conectará mediante SFTP para subir los archivos.</t>
+  </si>
+  <si>
+    <t>SFTPPort</t>
+  </si>
+  <si>
+    <t>Puerto a través del que se conectará al Host del cliente mediante SFTP.</t>
+  </si>
+  <si>
+    <t>SFTPCredentials</t>
+  </si>
+  <si>
+    <t>Nombre del Asset en el que estarán almacenadas las credenciales para conectar al servidor SFTP.</t>
+  </si>
+  <si>
+    <t>OrchestratorFolder</t>
+  </si>
+  <si>
+    <t>Carpeta del Orquestador en el que estarán los Assets.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -200,6 +224,13 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -226,16 +257,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -251,6 +283,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -632,7 +668,7 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -640,7 +676,7 @@
       </c>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C8" t="s">
@@ -658,11 +694,42 @@
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1646,6 +1713,8 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se completa el módulo UploadFiles
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webersolutionsespana-my.sharepoint.com/personal/jgonzalez_rpatechnologies_es/Documents/Documentos/UiPath/AVO_001_0300_Exportar_Facturas/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\AVO_001_0300_Exportar_Facturas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5700A415-4604-4AFA-A2D7-D48FB3662746}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF504D8-B5F7-4ED9-AB42-B8664816347B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -159,24 +159,6 @@
     <t>AVO_001_0300_Exportar_Facturas</t>
   </si>
   <si>
-    <t>PDFDestinationPath</t>
-  </si>
-  <si>
-    <t>XMLDestinationPath</t>
-  </si>
-  <si>
-    <t>PDFOriginPath</t>
-  </si>
-  <si>
-    <t>Ruta donde se almacena el documento original de la factura</t>
-  </si>
-  <si>
-    <t>Ruta donde se almacenará el documento PDF en los sistemas del cliente</t>
-  </si>
-  <si>
-    <t>Ruta donde se almacenará el documento XML generado</t>
-  </si>
-  <si>
     <t>SFTPHost</t>
   </si>
   <si>
@@ -199,6 +181,45 @@
   </si>
   <si>
     <t>Carpeta del Orquestador en el que estarán los Assets.</t>
+  </si>
+  <si>
+    <t>Ruta donde se almacenarán los ficheros a la espera de que se suban al servidor</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>Data\Temp\</t>
+  </si>
+  <si>
+    <t>TempFolder</t>
+  </si>
+  <si>
+    <t>RemoteFolder</t>
+  </si>
+  <si>
+    <t>Ruta donde se almacenará el documento en los sistemas del cliente</t>
+  </si>
+  <si>
+    <t>AVO_001</t>
+  </si>
+  <si>
+    <t>FolderOk</t>
+  </si>
+  <si>
+    <t>FolderKo</t>
+  </si>
+  <si>
+    <t>Ruta donde se almacenarán los ficheros XML que se han podido subir correctamente</t>
+  </si>
+  <si>
+    <t>Ruta donde se almacenarán los ficehros XML que no se han podido subir</t>
+  </si>
+  <si>
+    <t>Data\Output\ResultOk</t>
+  </si>
+  <si>
+    <t>Data\Output\ResultKo</t>
   </si>
 </sst>
 </file>
@@ -586,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -669,84 +690,115 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26">
       <c r="A7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
-      <c r="A8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:26">
-      <c r="A9" t="s">
-        <v>45</v>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>55</v>
+      <c r="C15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B19" s="2"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1713,8 +1765,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1727,7 +1777,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>